<commit_message>
TestFormation and TestTeams passing
</commit_message>
<xml_diff>
--- a/board.xlsx
+++ b/board.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="6">
   <si>
     <t>O</t>
   </si>
@@ -29,12 +29,18 @@
   <si>
     <t>C</t>
   </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +77,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -149,6 +160,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -183,6 +195,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -358,23 +371,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG14" sqref="A1:XFD1048576"/>
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="11" width="2.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="26" width="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.140625" customWidth="1"/>
     <col min="28" max="29" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -450,14 +463,17 @@
       <c r="Z1">
         <v>24</v>
       </c>
+      <c r="AA1">
+        <v>25</v>
+      </c>
       <c r="AB1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AC1">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -546,7 +562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -635,7 +651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -724,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -813,7 +829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -902,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -991,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1080,7 +1096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1169,7 +1185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1258,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1347,7 +1363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1355,7 +1371,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
         <v>2</v>
@@ -1430,13 +1446,13 @@
         <v>2</v>
       </c>
       <c r="AB12" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AC12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1444,7 +1460,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
         <v>2</v>
@@ -1519,13 +1535,13 @@
         <v>2</v>
       </c>
       <c r="AB13" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AC13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1614,7 +1630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1703,7 +1719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1792,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1881,7 +1897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1970,7 +1986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2059,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2148,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2237,7 +2253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2326,7 +2342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2422,24 +2438,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>